<commit_message>
Final commit with only my registration as user
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,172 +615,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>
@@ -795,7 +630,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -986,172 +821,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>
@@ -1166,7 +836,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF13"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1347,172 +1017,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>
@@ -1527,7 +1032,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1718,172 +1223,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>
@@ -1898,7 +1238,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2074,172 +1414,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>
@@ -2254,7 +1429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2445,172 +1620,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>
@@ -2625,7 +1635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF13"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2806,172 +1816,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>
@@ -2986,7 +1831,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3177,187 +2022,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>
@@ -3372,7 +2037,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF13"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3553,172 +2218,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>
@@ -3733,7 +2233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3924,172 +2424,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>
@@ -4104,7 +2439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4295,172 +2630,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>
@@ -4475,7 +2645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF13"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4656,172 +2826,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Suchitra Kushwaha</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2001066</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Vimla</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2001054</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ayush</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2001078</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pika</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001063</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>raju</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001064</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2001049</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pooja</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2001018</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Rohan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001034</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vikas</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001044</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sakshi</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2001011</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dinesh</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2001077</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Riya</t>
+          <t>Suchitra</t>
         </is>
       </c>
     </row>

</xml_diff>